<commit_message>
removed column names capital letters
</commit_message>
<xml_diff>
--- a/data_2023/SALMA.xlsx
+++ b/data_2023/SALMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63425AAE-D11C-4443-8851-7547A013B378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A93A10C-300C-45A1-939D-4F2CB0009865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{04C64777-6055-495D-8002-BBD1BCB13666}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
-    <t>Interval_name</t>
-  </si>
-  <si>
     <t>min_ma</t>
   </si>
   <si>
@@ -37,9 +34,6 @@
   </si>
   <si>
     <t>Lujanian</t>
-  </si>
-  <si>
-    <t>Epoch</t>
   </si>
   <si>
     <t>Pleistocene</t>
@@ -142,6 +136,12 @@
       </rPr>
       <t xml:space="preserve"> Zone</t>
     </r>
+  </si>
+  <si>
+    <t>epoch</t>
+  </si>
+  <si>
+    <t>interval_name</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,24 +534,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -562,10 +562,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -576,10 +576,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -590,10 +590,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -618,10 +618,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>5.3330000000000002</v>
@@ -632,10 +632,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>8</v>
@@ -646,10 +646,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2">
         <v>10</v>
@@ -660,10 +660,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2">
         <v>11.5</v>
@@ -674,10 +674,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>14</v>
@@ -688,10 +688,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2">
         <v>16</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2">
         <v>20</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
         <v>23.03</v>
@@ -730,10 +730,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2">
         <v>30</v>
@@ -744,10 +744,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2">
         <v>36</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C17" s="2">
         <v>39.5</v>
@@ -772,10 +772,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2">
         <v>44</v>
@@ -786,10 +786,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2">
         <v>47</v>
@@ -800,10 +800,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2">
         <v>50</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2">
         <v>51</v>
@@ -828,10 +828,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2">
         <v>59.2</v>
@@ -842,10 +842,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2">
         <v>62</v>
@@ -856,10 +856,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C24" s="2">
         <v>64</v>

</xml_diff>